<commit_message>
finished implementing the turning control mechanism.
</commit_message>
<xml_diff>
--- a/Robot Documentation.xlsx
+++ b/Robot Documentation.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David-Michael\Desktop\Mercury-2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\GitHub\Mercury-2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="4548" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Servo Positions" sheetId="1" r:id="rId1"/>
@@ -198,10 +198,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,17 +519,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -537,308 +537,308 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1223</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>1441</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>1876</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>2416</v>
       </c>
       <c r="H5" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1812</v>
       </c>
-      <c r="D6" s="3">
-        <v>1588</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="2">
+        <v>1520</v>
+      </c>
+      <c r="E6" s="2">
         <v>1065</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>542</v>
       </c>
       <c r="H6" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>1746</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>1510</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>1026</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>533</v>
       </c>
       <c r="H7" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>1185</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>1425</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>1185</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>2400</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="H10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>1504</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>944</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="H11" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
       <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>2000</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>800</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="H12" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>2496</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>646</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
       <c r="H13" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>2496</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>646</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="H14" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="2"/>
       <c r="H16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>2000</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>1000</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>1500</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="2"/>
       <c r="H17" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
       <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>2000</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>1000</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>1500</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="2"/>
       <c r="H18" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
       <c r="H20" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>4000</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>64</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
       <c r="H21" s="1">
         <v>6</v>
       </c>
@@ -857,22 +857,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>29</v>
       </c>
@@ -880,7 +880,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -888,7 +888,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>32</v>
       </c>
@@ -896,7 +896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>33</v>
       </c>
@@ -904,7 +904,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>34</v>
       </c>
@@ -912,7 +912,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>35</v>
       </c>
@@ -920,7 +920,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>36</v>
       </c>
@@ -928,7 +928,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>37</v>
       </c>

</xml_diff>